<commit_message>
Updated PSD excel sheet
</commit_message>
<xml_diff>
--- a/Data/psd-and-averages.xlsx
+++ b/Data/psd-and-averages.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\autum\Sites\AquaMachina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3B4764-001B-43D9-913D-F41975B57F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8717BC2-EF9C-4F5E-9957-4119F595B63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{562F5B8B-2852-46D8-B8B0-3B22FB8729BD}"/>
+    <workbookView xWindow="9525" yWindow="0" windowWidth="9750" windowHeight="10155" activeTab="1" xr2:uid="{562F5B8B-2852-46D8-B8B0-3B22FB8729BD}"/>
   </bookViews>
   <sheets>
     <sheet name="PSD" sheetId="1" r:id="rId1"/>
+    <sheet name="alt-chart-design" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>d_p (um)</t>
   </si>
@@ -46,13 +47,22 @@
   <si>
     <t>Average</t>
   </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>d_p</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -85,10 +95,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,7 +192,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.2512749409360966E-2"/>
+          <c:y val="0.13215767625486383"/>
+          <c:w val="0.92472064923206687"/>
+          <c:h val="0.65687880633786444"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -298,7 +318,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -393,7 +413,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent3">
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -489,6 +509,8 @@
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -583,7 +605,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -678,7 +702,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -773,7 +799,8 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -872,7 +899,8 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -971,7 +999,8 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="10000"/>
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -1071,6 +1100,7 @@
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -1166,7 +1196,8 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -1265,7 +1296,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent3">
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -1364,7 +1395,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent4">
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -1465,7 +1496,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -1566,7 +1597,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent6">
                   <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -1665,11 +1696,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="90000"/>
+                  <a:lumOff val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1678,19 +1709,19 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="90000"/>
+                  <a:lumOff val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="80000"/>
-                    <a:lumOff val="20000"/>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="90000"/>
+                    <a:lumOff val="10000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -2093,7 +2124,750 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Particle Size</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Distribution Range for the 15 Storm Events Studied</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'alt-chart-design'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'alt-chart-design'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'alt-chart-design'!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E7AC-4C7F-A093-B0A05324B171}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'alt-chart-design'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'alt-chart-design'!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>158.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>573.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'alt-chart-design'!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E7AC-4C7F-A093-B0A05324B171}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'alt-chart-design'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'alt-chart-design'!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>956</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'alt-chart-design'!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E7AC-4C7F-A093-B0A05324B171}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1291556159"/>
+        <c:axId val="1710720111"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1291556159"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="maxMin"/>
+          <c:max val="2000"/>
+          <c:min val="2.0000000000000004E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Particle Diameter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" baseline="0"/>
+                  <a:t>μ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>m)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1710720111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1710720111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% Finer by Mass</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1291556159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2649,20 +3423,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>90486</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>187324</xdr:rowOff>
+      <xdr:colOff>96836</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>12699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>511175</xdr:colOff>
+      <xdr:colOff>517525</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2670,6 +3960,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A17951-E60E-7A90-FE2B-ECFAEF3B4F2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>207962</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>68262</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3601D4C-D57D-927B-1AED-E5789A37369C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3009,8 +4340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1E778A-C130-4A4E-8FB4-25138F57150C}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:Q7"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3027,71 +4358,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.75">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>39527</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>39584</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>39602</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>39609</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>39620</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>39637</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>39644</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>39658</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>39668</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>39672</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>39679</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>39701</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>39711</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>39729</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>39744</v>
       </c>
       <c r="Q2" t="s">
@@ -3370,7 +4702,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3378,4 +4710,136 @@
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8FAD3E-BD8E-4FCA-B2D5-FE18E3B2CB53}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>MIN(PSD!B3:P3)</f>
+        <v>0.02</v>
+      </c>
+      <c r="C3">
+        <f>PSD!Q3</f>
+        <v>0.02</v>
+      </c>
+      <c r="D3">
+        <f>MAX(PSD!B3:P3)</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <f>MIN(PSD!B4:P4)</f>
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <f>PSD!Q4</f>
+        <v>36.333333333333336</v>
+      </c>
+      <c r="D4">
+        <f>MAX(PSD!B4:P4)</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <f>MIN(PSD!B5:P5)</f>
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <f>PSD!Q5</f>
+        <v>158.4</v>
+      </c>
+      <c r="D5">
+        <f>MAX(PSD!B5:P5)</f>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>85</v>
+      </c>
+      <c r="B6">
+        <f>MIN(PSD!B6:P6)</f>
+        <v>219</v>
+      </c>
+      <c r="C6">
+        <f>PSD!Q6</f>
+        <v>573.33333333333337</v>
+      </c>
+      <c r="D6">
+        <f>MAX(PSD!B6:P6)</f>
+        <v>956</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <f>MIN(PSD!B7:P7)</f>
+        <v>2000</v>
+      </c>
+      <c r="C7">
+        <f>PSD!Q7</f>
+        <v>2000</v>
+      </c>
+      <c r="D7">
+        <f>MAX(PSD!B7:P7)</f>
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B3:B7 D3:D7" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>